<commit_message>
export import inventaris, paket, letakserver done
</commit_message>
<xml_diff>
--- a/bootstrap/paketexport (2).xlsx
+++ b/bootstrap/paketexport (2).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>No</t>
   </si>
@@ -38,13 +38,10 @@
     <t>Paket Breton</t>
   </si>
   <si>
-    <t>2021-04-26T15:33:10.000000Z</t>
+    <t>2021-05-03T14:53:17.000000Z</t>
   </si>
   <si>
     <t>Paket Toussaint</t>
-  </si>
-  <si>
-    <t>2021-04-26T15:33:11.000000Z</t>
   </si>
   <si>
     <t>Paket Masson-les-Bains</t>
@@ -457,7 +454,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -477,7 +474,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -489,18 +486,18 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>45000</v>
@@ -509,18 +506,18 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>25000</v>
@@ -529,18 +526,18 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>55000</v>
@@ -549,18 +546,18 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>55000</v>
@@ -569,18 +566,18 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>100000</v>
@@ -589,18 +586,18 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>65000</v>
@@ -609,18 +606,18 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>10000</v>
@@ -629,18 +626,18 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>50000</v>
@@ -649,10 +646,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>